<commit_message>
Updated Standings, Box Scores, Playoffs
Data Input to EOD 4/16/25,
Updated Playoff Brackets, Box Scores
</commit_message>
<xml_diff>
--- a/2024_2025/Playoffs/Brackets.xlsx
+++ b/2024_2025/Playoffs/Brackets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\Templates\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024_2025\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9671C46C-9EE8-4F83-8D98-49A640B312EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0465FDB8-C5AC-442B-8A18-68A475C6C541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="48">
   <si>
     <t>Eastern Conference Playoff Teams</t>
   </si>
@@ -73,24 +73,6 @@
     <t>1st Round</t>
   </si>
   <si>
-    <t>1 vs 8</t>
-  </si>
-  <si>
-    <t>2 vs 7</t>
-  </si>
-  <si>
-    <t>3 vs 6</t>
-  </si>
-  <si>
-    <t>4 vs 5</t>
-  </si>
-  <si>
-    <t>1 vs 8 Winner vs 3 vs 6 Winner</t>
-  </si>
-  <si>
-    <t>2 vs 7 Winner vs 4 vs 5 Winner</t>
-  </si>
-  <si>
     <t>2nd Round</t>
   </si>
   <si>
@@ -106,31 +88,88 @@
     <t>Conference Winners</t>
   </si>
   <si>
-    <t>1st Place vs 8th Place</t>
-  </si>
-  <si>
-    <t>3rd Place vs 6th Place</t>
-  </si>
-  <si>
-    <t>4th Place vs 5th Place</t>
-  </si>
-  <si>
-    <t>2nd Place vs 7th Place</t>
-  </si>
-  <si>
     <t>Round 2</t>
   </si>
   <si>
-    <t>1st/8th Place Winner vs 3rd/6th Place Winner</t>
-  </si>
-  <si>
-    <t>2nd/7th Place Winner vs 4th/5th Place Winner</t>
-  </si>
-  <si>
     <t>NHL Finals</t>
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Carolina Hurricanes</t>
+  </si>
+  <si>
+    <t>Florida Panthers</t>
+  </si>
+  <si>
+    <t>Montreal Canadiens</t>
+  </si>
+  <si>
+    <t>New Jersey Devils</t>
+  </si>
+  <si>
+    <t>Ottawa Senators</t>
+  </si>
+  <si>
+    <t>Tampa Bay Lightning</t>
+  </si>
+  <si>
+    <t>Toronto Maple Leafs</t>
+  </si>
+  <si>
+    <t>Washington Capitals</t>
+  </si>
+  <si>
+    <t>Colorado Avalanche</t>
+  </si>
+  <si>
+    <t>Dallas Stars</t>
+  </si>
+  <si>
+    <t>Edmonton Oilers</t>
+  </si>
+  <si>
+    <t>Los Angeles Kings</t>
+  </si>
+  <si>
+    <t>Minnesota Wild</t>
+  </si>
+  <si>
+    <t>St. Louis Blues</t>
+  </si>
+  <si>
+    <t>Vegas Golden Knights</t>
+  </si>
+  <si>
+    <t>Winnipeg Jets</t>
+  </si>
+  <si>
+    <t>1 vs 4</t>
+  </si>
+  <si>
+    <t>2 vs 3</t>
+  </si>
+  <si>
+    <t>1 vs 4 Winner vs 2 vs 3 Winner</t>
+  </si>
+  <si>
+    <t>1st Place vs 4th Place</t>
+  </si>
+  <si>
+    <t>2nd Place vs 3rd Place</t>
+  </si>
+  <si>
+    <t>1st/4th Place Winner vs 2nd/3rd Place Winner</t>
+  </si>
+  <si>
+    <t>5*</t>
+  </si>
+  <si>
+    <t>6*</t>
+  </si>
+  <si>
+    <t>7*</t>
   </si>
 </sst>
 </file>
@@ -384,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -509,13 +548,43 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -536,35 +605,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -848,18 +893,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37.42578125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -871,23 +916,99 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="44"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="42"/>
       <c r="G11" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -910,87 +1031,122 @@
         <v>5</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="43"/>
+      <c r="A13" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="44"/>
+      <c r="C13" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="44"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="43"/>
+      <c r="A16" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="44"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="43"/>
+      <c r="A19" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="44"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="43"/>
+      <c r="A22" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="44"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="7:12" x14ac:dyDescent="0.25">
@@ -1056,17 +1212,31 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14:A15 A17:A18 A20:A21 A23:A24" xr:uid="{65B733ED-E905-4ECB-B300-CE3F9293197B}">
+      <formula1>$A$2:$A$9</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:B15 B17:B18 B20:B21 B23:B24" xr:uid="{CB570C17-010C-4F8A-ABC2-C4F9FB9794D3}">
+      <formula1>$B$2:$B$9</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C15 C17:C18" xr:uid="{7B11D81C-FC3F-46CB-BC09-BE0206DCB418}">
+      <formula1>$C$2:$C$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D15 D17:D18" xr:uid="{EB0ED61F-2A9C-4FA6-BD7B-7ED0CBBF83D1}">
+      <formula1>$D$2:$D$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1076,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,131 +1294,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="Z1" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="55"/>
-      <c r="AF1" s="53" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="54"/>
+      <c r="Z1" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="54"/>
+      <c r="AF1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
-      <c r="AX1" s="54"/>
-      <c r="AY1" s="54"/>
-      <c r="AZ1" s="54"/>
-      <c r="BA1" s="55"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="53"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="54"/>
     </row>
     <row r="2" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
-      <c r="M2" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="59"/>
-      <c r="AI2" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ2" s="58"/>
-      <c r="AK2" s="58"/>
-      <c r="AL2" s="58"/>
-      <c r="AM2" s="58"/>
-      <c r="AN2" s="58"/>
-      <c r="AO2" s="59"/>
-      <c r="AU2" s="57" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="M2" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="50"/>
+      <c r="AI2" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="50"/>
+      <c r="AU2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AV2" s="58"/>
-      <c r="AW2" s="58"/>
-      <c r="AX2" s="58"/>
-      <c r="AY2" s="58"/>
-      <c r="AZ2" s="58"/>
-      <c r="BA2" s="59"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="49"/>
+      <c r="AY2" s="49"/>
+      <c r="AZ2" s="49"/>
+      <c r="BA2" s="50"/>
     </row>
     <row r="3" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="AI3" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="51"/>
-      <c r="AN3" s="51"/>
-      <c r="AO3" s="51"/>
-      <c r="AU3" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="AV3" s="51"/>
-      <c r="AW3" s="51"/>
-      <c r="AX3" s="51"/>
-      <c r="AY3" s="51"/>
-      <c r="AZ3" s="51"/>
-      <c r="BA3" s="51"/>
+      <c r="A3" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="AI3" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="57"/>
+      <c r="AU3" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV3" s="45"/>
+      <c r="AW3" s="45"/>
+      <c r="AX3" s="45"/>
+      <c r="AY3" s="45"/>
+      <c r="AZ3" s="45"/>
+      <c r="BA3" s="45"/>
     </row>
     <row r="4" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -1265,20 +1435,20 @@
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="47"/>
+      <c r="M4" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="57"/>
       <c r="AI4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>3</v>
@@ -1299,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="AV4" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="AW4" s="3" t="s">
         <v>3</v>
@@ -1321,17 +1491,23 @@
       <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="26">
+        <v>45767</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="5"/>
       <c r="M5" s="22" t="s">
         <v>2</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="O5" s="22" t="s">
         <v>3</v>
@@ -1360,10 +1536,16 @@
       <c r="AU5" s="7">
         <v>1</v>
       </c>
-      <c r="AV5" s="26"/>
-      <c r="AW5" s="10"/>
+      <c r="AV5" s="26">
+        <v>45766</v>
+      </c>
+      <c r="AW5" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="AX5" s="11"/>
-      <c r="AY5" s="10"/>
+      <c r="AY5" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="AZ5" s="11"/>
       <c r="BA5" s="5"/>
     </row>
@@ -1371,10 +1553,16 @@
       <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="27">
+        <v>45769</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="16"/>
       <c r="M6" s="7">
@@ -1398,10 +1586,16 @@
       <c r="AU6" s="8">
         <v>2</v>
       </c>
-      <c r="AV6" s="27"/>
-      <c r="AW6" s="12"/>
+      <c r="AV6" s="27">
+        <v>45768</v>
+      </c>
+      <c r="AW6" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="AX6" s="13"/>
-      <c r="AY6" s="12"/>
+      <c r="AY6" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="AZ6" s="13"/>
       <c r="BA6" s="16"/>
     </row>
@@ -1409,10 +1603,16 @@
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="27">
+        <v>45771</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="16"/>
       <c r="M7" s="8">
@@ -1436,10 +1636,16 @@
       <c r="AU7" s="8">
         <v>3</v>
       </c>
-      <c r="AV7" s="27"/>
-      <c r="AW7" s="12"/>
+      <c r="AV7" s="27">
+        <v>45771</v>
+      </c>
+      <c r="AW7" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="AX7" s="13"/>
-      <c r="AY7" s="12"/>
+      <c r="AY7" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="AZ7" s="13"/>
       <c r="BA7" s="16"/>
     </row>
@@ -1447,15 +1653,21 @@
       <c r="A8" s="8">
         <v>4</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="27">
+        <v>45773</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="16"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
@@ -1474,27 +1686,39 @@
       <c r="AM8" s="30"/>
       <c r="AN8" s="31"/>
       <c r="AO8" s="16"/>
-      <c r="AQ8" s="52"/>
-      <c r="AR8" s="52"/>
-      <c r="AS8" s="52"/>
+      <c r="AQ8" s="46"/>
+      <c r="AR8" s="46"/>
+      <c r="AS8" s="46"/>
       <c r="AU8" s="38">
         <v>4</v>
       </c>
-      <c r="AV8" s="33"/>
-      <c r="AW8" s="30"/>
+      <c r="AV8" s="33">
+        <v>45774</v>
+      </c>
+      <c r="AW8" s="30" t="s">
+        <v>38</v>
+      </c>
       <c r="AX8" s="31"/>
-      <c r="AY8" s="30"/>
+      <c r="AY8" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="AZ8" s="31"/>
       <c r="BA8" s="32"/>
     </row>
     <row r="9" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B9" s="27">
+        <v>45776</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="D9" s="13"/>
-      <c r="E9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" s="13"/>
       <c r="G9" s="16"/>
       <c r="L9" s="12"/>
@@ -1508,7 +1732,7 @@
       <c r="R9" s="13"/>
       <c r="S9" s="16"/>
       <c r="AI9" s="8" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="AJ9" s="27"/>
       <c r="AK9" s="12"/>
@@ -1520,28 +1744,40 @@
       <c r="AR9" s="17"/>
       <c r="AS9" s="17"/>
       <c r="AU9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV9" s="27"/>
-      <c r="AW9" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="AV9" s="27">
+        <v>45777</v>
+      </c>
+      <c r="AW9" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="AX9" s="13"/>
-      <c r="AY9" s="12"/>
+      <c r="AY9" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="AZ9" s="13"/>
       <c r="BA9" s="32"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="B10" s="27">
+        <v>45778</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F10" s="13"/>
       <c r="G10" s="16"/>
       <c r="L10" s="12"/>
       <c r="M10" s="8" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="N10" s="33"/>
       <c r="O10" s="12"/>
@@ -1550,7 +1786,7 @@
       <c r="R10" s="13"/>
       <c r="S10" s="16"/>
       <c r="AI10" s="8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="AJ10" s="27"/>
       <c r="AK10" s="12"/>
@@ -1560,28 +1796,40 @@
       <c r="AO10" s="16"/>
       <c r="AQ10" s="12"/>
       <c r="AU10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AV10" s="27"/>
-      <c r="AW10" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="AV10" s="27">
+        <v>45779</v>
+      </c>
+      <c r="AW10" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="AX10" s="13"/>
-      <c r="AY10" s="12"/>
+      <c r="AY10" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="AZ10" s="13"/>
       <c r="BA10" s="16"/>
     </row>
     <row r="11" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="B11" s="28">
+        <v>45780</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="D11" s="15"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="F11" s="15"/>
       <c r="G11" s="6"/>
       <c r="L11" s="12"/>
       <c r="M11" s="8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="N11" s="33"/>
       <c r="O11" s="12"/>
@@ -1590,7 +1838,7 @@
       <c r="R11" s="13"/>
       <c r="S11" s="16"/>
       <c r="AI11" s="9" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="AJ11" s="28"/>
       <c r="AK11" s="14"/>
@@ -1600,28 +1848,34 @@
       <c r="AO11" s="6"/>
       <c r="AQ11" s="12"/>
       <c r="AU11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV11" s="28"/>
-      <c r="AW11" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="AV11" s="28">
+        <v>45781</v>
+      </c>
+      <c r="AW11" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="AX11" s="15"/>
-      <c r="AY11" s="14"/>
+      <c r="AY11" s="14" t="s">
+        <v>38</v>
+      </c>
       <c r="AZ11" s="15"/>
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="L12" s="12"/>
-      <c r="M12" s="8" t="s">
-        <v>12</v>
+      <c r="M12" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="12"/>
@@ -1629,72 +1883,72 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="51" t="s">
+      <c r="AI12" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AJ12" s="51"/>
-      <c r="AK12" s="51"/>
-      <c r="AL12" s="51"/>
-      <c r="AM12" s="51"/>
-      <c r="AN12" s="51"/>
-      <c r="AO12" s="51"/>
+      <c r="AJ12" s="45"/>
+      <c r="AK12" s="45"/>
+      <c r="AL12" s="45"/>
+      <c r="AM12" s="45"/>
+      <c r="AN12" s="45"/>
+      <c r="AO12" s="45"/>
       <c r="AQ12" s="12"/>
-      <c r="AU12" s="51" t="s">
+      <c r="AU12" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AV12" s="51"/>
-      <c r="AW12" s="51"/>
-      <c r="AX12" s="51"/>
-      <c r="AY12" s="51"/>
-      <c r="AZ12" s="51"/>
-      <c r="BA12" s="51"/>
+      <c r="AV12" s="45"/>
+      <c r="AW12" s="45"/>
+      <c r="AX12" s="45"/>
+      <c r="AY12" s="45"/>
+      <c r="AZ12" s="45"/>
+      <c r="BA12" s="45"/>
     </row>
     <row r="13" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="47"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="56"/>
+      <c r="S13" s="57"/>
       <c r="AQ13" s="12"/>
     </row>
     <row r="14" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="AN14" s="52"/>
-      <c r="AO14" s="52"/>
-      <c r="AP14" s="52"/>
+      <c r="A14" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="AN14" s="46"/>
+      <c r="AO14" s="46"/>
+      <c r="AP14" s="46"/>
       <c r="AQ14" s="12"/>
-      <c r="AU14" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="AV14" s="51"/>
-      <c r="AW14" s="51"/>
-      <c r="AX14" s="51"/>
-      <c r="AY14" s="51"/>
-      <c r="AZ14" s="51"/>
-      <c r="BA14" s="51"/>
+      <c r="AU14" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV14" s="62"/>
+      <c r="AW14" s="62"/>
+      <c r="AX14" s="62"/>
+      <c r="AY14" s="62"/>
+      <c r="AZ14" s="62"/>
+      <c r="BA14" s="62"/>
     </row>
     <row r="15" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>3</v>
@@ -1719,7 +1973,7 @@
         <v>2</v>
       </c>
       <c r="AV15" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="AW15" s="3" t="s">
         <v>3</v>
@@ -1741,10 +1995,16 @@
       <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="26">
+        <v>45769</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="5"/>
       <c r="L16" s="12"/>
@@ -1754,10 +2014,16 @@
       <c r="AU16" s="7">
         <v>1</v>
       </c>
-      <c r="AV16" s="26"/>
-      <c r="AW16" s="10"/>
+      <c r="AV16" s="26">
+        <v>45766</v>
+      </c>
+      <c r="AW16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="AX16" s="11"/>
-      <c r="AY16" s="10"/>
+      <c r="AY16" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="AZ16" s="11"/>
       <c r="BA16" s="5"/>
     </row>
@@ -1765,10 +2031,16 @@
       <c r="A17" s="8">
         <v>2</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="27">
+        <v>45771</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="F17" s="13"/>
       <c r="G17" s="16"/>
       <c r="L17" s="12"/>
@@ -1778,10 +2050,16 @@
       <c r="AU17" s="8">
         <v>2</v>
       </c>
-      <c r="AV17" s="27"/>
-      <c r="AW17" s="12"/>
+      <c r="AV17" s="27">
+        <v>45768</v>
+      </c>
+      <c r="AW17" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="AX17" s="13"/>
-      <c r="AY17" s="12"/>
+      <c r="AY17" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="AZ17" s="13"/>
       <c r="BA17" s="16"/>
     </row>
@@ -1789,10 +2067,16 @@
       <c r="A18" s="8">
         <v>3</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="27">
+        <v>45773</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="D18" s="13"/>
-      <c r="E18" s="12"/>
+      <c r="E18" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="F18" s="13"/>
       <c r="G18" s="16"/>
       <c r="L18" s="12"/>
@@ -1802,10 +2086,16 @@
       <c r="AU18" s="8">
         <v>3</v>
       </c>
-      <c r="AV18" s="27"/>
-      <c r="AW18" s="12"/>
+      <c r="AV18" s="27">
+        <v>45770</v>
+      </c>
+      <c r="AW18" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="AX18" s="13"/>
-      <c r="AY18" s="12"/>
+      <c r="AY18" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="AZ18" s="13"/>
       <c r="BA18" s="16"/>
     </row>
@@ -1813,151 +2103,199 @@
       <c r="A19" s="8">
         <v>4</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="30"/>
+      <c r="B19" s="33">
+        <v>45775</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="D19" s="31"/>
-      <c r="E19" s="30"/>
+      <c r="E19" s="30" t="s">
+        <v>24</v>
+      </c>
       <c r="F19" s="31"/>
       <c r="G19" s="32"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="56"/>
-      <c r="AR19" s="52"/>
-      <c r="AS19" s="52"/>
+      <c r="AQ19" s="47"/>
+      <c r="AR19" s="46"/>
+      <c r="AS19" s="46"/>
       <c r="AU19" s="38">
         <v>4</v>
       </c>
-      <c r="AV19" s="33"/>
-      <c r="AW19" s="30"/>
+      <c r="AV19" s="33">
+        <v>45773</v>
+      </c>
+      <c r="AW19" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="AX19" s="31"/>
-      <c r="AY19" s="30"/>
+      <c r="AY19" s="30" t="s">
+        <v>31</v>
+      </c>
       <c r="AZ19" s="31"/>
       <c r="BA19" s="32"/>
     </row>
     <row r="20" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B20" s="27">
+        <v>45777</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="F20" s="13"/>
       <c r="G20" s="16"/>
       <c r="O20" s="12"/>
       <c r="AN20" s="12"/>
       <c r="AU20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV20" s="27"/>
-      <c r="AW20" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="AV20" s="27">
+        <v>45775</v>
+      </c>
+      <c r="AW20" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="AX20" s="13"/>
-      <c r="AY20" s="12"/>
+      <c r="AY20" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="AZ20" s="13"/>
       <c r="BA20" s="16"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="B21" s="27">
+        <v>45779</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
+      <c r="E21" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="F21" s="13"/>
       <c r="G21" s="16"/>
       <c r="O21" s="12"/>
       <c r="AN21" s="12"/>
       <c r="AU21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AV21" s="27"/>
-      <c r="AW21" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="AV21" s="27">
+        <v>45778</v>
+      </c>
+      <c r="AW21" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="AX21" s="13"/>
-      <c r="AY21" s="12"/>
+      <c r="AY21" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="AZ21" s="13"/>
       <c r="BA21" s="16"/>
     </row>
     <row r="22" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="B22" s="28">
+        <v>45781</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="D22" s="15"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F22" s="15"/>
       <c r="G22" s="6"/>
       <c r="O22" s="12"/>
       <c r="AN22" s="12"/>
       <c r="AU22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV22" s="28"/>
-      <c r="AW22" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="AV22" s="28">
+        <v>45780</v>
+      </c>
+      <c r="AW22" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="AX22" s="15"/>
-      <c r="AY22" s="14"/>
+      <c r="AY22" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="AZ22" s="15"/>
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="51" t="s">
+      <c r="AU23" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AV23" s="51"/>
-      <c r="AW23" s="51"/>
-      <c r="AX23" s="51"/>
-      <c r="AY23" s="51"/>
-      <c r="AZ23" s="51"/>
-      <c r="BA23" s="51"/>
+      <c r="AV23" s="45"/>
+      <c r="AW23" s="45"/>
+      <c r="AX23" s="45"/>
+      <c r="AY23" s="45"/>
+      <c r="AZ23" s="45"/>
+      <c r="BA23" s="45"/>
     </row>
     <row r="24" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
+      <c r="A25" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="AV25" s="51"/>
-      <c r="AW25" s="51"/>
-      <c r="AX25" s="51"/>
-      <c r="AY25" s="51"/>
-      <c r="AZ25" s="51"/>
-      <c r="BA25" s="51"/>
+      <c r="AU25" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV25" s="45"/>
+      <c r="AW25" s="45"/>
+      <c r="AX25" s="45"/>
+      <c r="AY25" s="45"/>
+      <c r="AZ25" s="45"/>
+      <c r="BA25" s="45"/>
     </row>
     <row r="26" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>3</v>
@@ -1974,29 +2312,29 @@
       <c r="G26" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="O26" s="56"/>
-      <c r="P26" s="52"/>
-      <c r="Q26" s="52"/>
-      <c r="R26" s="52"/>
-      <c r="S26" s="52"/>
-      <c r="T26" s="52"/>
-      <c r="U26" s="52"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="52"/>
-      <c r="AE26" s="52"/>
-      <c r="AF26" s="52"/>
-      <c r="AG26" s="52"/>
-      <c r="AH26" s="52"/>
-      <c r="AI26" s="52"/>
-      <c r="AJ26" s="52"/>
-      <c r="AK26" s="52"/>
-      <c r="AL26" s="52"/>
-      <c r="AM26" s="60"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="46"/>
+      <c r="AE26" s="46"/>
+      <c r="AF26" s="46"/>
+      <c r="AG26" s="46"/>
+      <c r="AH26" s="46"/>
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="46"/>
+      <c r="AK26" s="46"/>
+      <c r="AL26" s="46"/>
+      <c r="AM26" s="51"/>
       <c r="AU26" s="20" t="s">
         <v>2</v>
       </c>
       <c r="AV26" s="20" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="AW26" s="20" t="s">
         <v>3</v>
@@ -2018,10 +2356,16 @@
       <c r="A27" s="7">
         <v>1</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="26">
+        <v>45768</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="D27" s="11"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="F27" s="11"/>
       <c r="G27" s="5"/>
       <c r="O27" s="12"/>
@@ -2031,10 +2375,16 @@
       <c r="AU27" s="7">
         <v>1</v>
       </c>
-      <c r="AV27" s="26"/>
-      <c r="AW27" s="10"/>
+      <c r="AV27" s="26">
+        <v>45767</v>
+      </c>
+      <c r="AW27" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="AX27" s="11"/>
-      <c r="AY27" s="10"/>
+      <c r="AY27" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="AZ27" s="11"/>
       <c r="BA27" s="5"/>
     </row>
@@ -2042,41 +2392,53 @@
       <c r="A28" s="8">
         <v>2</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="27">
+        <v>45770</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="12"/>
+      <c r="E28" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="F28" s="13"/>
       <c r="G28" s="16"/>
       <c r="O28" s="12"/>
-      <c r="P28" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="46"/>
-      <c r="V28" s="47"/>
+      <c r="P28" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="56"/>
+      <c r="V28" s="57"/>
       <c r="X28" s="12"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
+      <c r="AF28" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG28" s="45"/>
+      <c r="AH28" s="45"/>
+      <c r="AI28" s="45"/>
+      <c r="AJ28" s="45"/>
+      <c r="AK28" s="45"/>
+      <c r="AL28" s="45"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
       </c>
-      <c r="AV28" s="27"/>
-      <c r="AW28" s="12"/>
+      <c r="AV28" s="27">
+        <v>45769</v>
+      </c>
+      <c r="AW28" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="AX28" s="13"/>
-      <c r="AY28" s="12"/>
+      <c r="AY28" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="AZ28" s="13"/>
       <c r="BA28" s="16"/>
     </row>
@@ -2084,10 +2446,16 @@
       <c r="A29" s="8">
         <v>3</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="12"/>
+      <c r="B29" s="27">
+        <v>45772</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="D29" s="13"/>
-      <c r="E29" s="12"/>
+      <c r="E29" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F29" s="13"/>
       <c r="G29" s="16"/>
       <c r="O29" s="12"/>
@@ -2095,7 +2463,7 @@
         <v>2</v>
       </c>
       <c r="Q29" s="22" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="R29" s="22" t="s">
         <v>3</v>
@@ -2118,7 +2486,7 @@
         <v>2</v>
       </c>
       <c r="AG29" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="AH29" s="3" t="s">
         <v>3</v>
@@ -2139,10 +2507,16 @@
       <c r="AU29" s="8">
         <v>3</v>
       </c>
-      <c r="AV29" s="27"/>
-      <c r="AW29" s="12"/>
+      <c r="AV29" s="27">
+        <v>45771</v>
+      </c>
+      <c r="AW29" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="AX29" s="13"/>
-      <c r="AY29" s="12"/>
+      <c r="AY29" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="AZ29" s="13"/>
       <c r="BA29" s="16"/>
     </row>
@@ -2150,15 +2524,21 @@
       <c r="A30" s="8">
         <v>4</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="30"/>
+      <c r="B30" s="33">
+        <v>45774</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="D30" s="31"/>
-      <c r="E30" s="30"/>
+      <c r="E30" s="30" t="s">
+        <v>25</v>
+      </c>
       <c r="F30" s="31"/>
       <c r="G30" s="32"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
@@ -2181,27 +2561,39 @@
       <c r="AK30" s="24"/>
       <c r="AL30" s="25"/>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="52"/>
-      <c r="AR30" s="52"/>
-      <c r="AS30" s="52"/>
+      <c r="AQ30" s="46"/>
+      <c r="AR30" s="46"/>
+      <c r="AS30" s="46"/>
       <c r="AU30" s="38">
         <v>4</v>
       </c>
-      <c r="AV30" s="33"/>
-      <c r="AW30" s="30"/>
+      <c r="AV30" s="33">
+        <v>45773</v>
+      </c>
+      <c r="AW30" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="AX30" s="31"/>
-      <c r="AY30" s="30"/>
+      <c r="AY30" s="30" t="s">
+        <v>35</v>
+      </c>
       <c r="AZ30" s="31"/>
       <c r="BA30" s="32"/>
     </row>
     <row r="31" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B31" s="27">
+        <v>45777</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="D31" s="13"/>
-      <c r="E31" s="12"/>
+      <c r="E31" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="F31" s="13"/>
       <c r="G31" s="32"/>
       <c r="L31" s="12"/>
@@ -2231,23 +2623,35 @@
       <c r="AR31" s="17"/>
       <c r="AS31" s="17"/>
       <c r="AU31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV31" s="27"/>
-      <c r="AW31" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="AV31" s="27">
+        <v>45776</v>
+      </c>
+      <c r="AW31" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="AX31" s="13"/>
-      <c r="AY31" s="12"/>
+      <c r="AY31" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="AZ31" s="13"/>
       <c r="BA31" s="16"/>
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="B32" s="27">
+        <v>45779</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F32" s="13"/>
       <c r="G32" s="16"/>
       <c r="L32" s="12"/>
@@ -2275,23 +2679,35 @@
       <c r="AN32" s="12"/>
       <c r="AQ32" s="12"/>
       <c r="AU32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AV32" s="27"/>
-      <c r="AW32" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="AV32" s="27">
+        <v>45778</v>
+      </c>
+      <c r="AW32" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="AX32" s="13"/>
-      <c r="AY32" s="12"/>
+      <c r="AY32" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="AZ32" s="13"/>
       <c r="BA32" s="16"/>
     </row>
     <row r="33" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="B33" s="28">
+        <v>45781</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="D33" s="15"/>
-      <c r="E33" s="14"/>
+      <c r="E33" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="F33" s="15"/>
       <c r="G33" s="6"/>
       <c r="L33" s="12"/>
@@ -2319,29 +2735,35 @@
       <c r="AN33" s="12"/>
       <c r="AQ33" s="12"/>
       <c r="AU33" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV33" s="28"/>
-      <c r="AW33" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="AV33" s="28">
+        <v>45780</v>
+      </c>
+      <c r="AW33" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="AX33" s="15"/>
-      <c r="AY33" s="14"/>
+      <c r="AY33" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="AZ33" s="15"/>
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="Q34" s="40"/>
       <c r="R34" s="12"/>
@@ -2352,7 +2774,7 @@
       <c r="X34" s="12"/>
       <c r="AD34" s="13"/>
       <c r="AF34" s="8" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="AG34" s="27"/>
       <c r="AH34" s="12"/>
@@ -2362,21 +2784,21 @@
       <c r="AL34" s="16"/>
       <c r="AN34" s="12"/>
       <c r="AQ34" s="12"/>
-      <c r="AU34" s="51" t="s">
+      <c r="AU34" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AV34" s="51"/>
-      <c r="AW34" s="51"/>
-      <c r="AX34" s="51"/>
-      <c r="AY34" s="51"/>
-      <c r="AZ34" s="51"/>
-      <c r="BA34" s="51"/>
+      <c r="AV34" s="45"/>
+      <c r="AW34" s="45"/>
+      <c r="AX34" s="45"/>
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
     </row>
     <row r="35" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
       <c r="O35" s="12"/>
       <c r="P35" s="8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="Q35" s="40"/>
       <c r="R35" s="12"/>
@@ -2387,7 +2809,7 @@
       <c r="X35" s="12"/>
       <c r="AD35" s="13"/>
       <c r="AF35" s="8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="AG35" s="27"/>
       <c r="AH35" s="12"/>
@@ -2399,21 +2821,21 @@
       <c r="AQ35" s="12"/>
     </row>
     <row r="36" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="52"/>
+      <c r="A36" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
       <c r="O36" s="12"/>
-      <c r="P36" s="8" t="s">
-        <v>12</v>
+      <c r="P36" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="Q36" s="41"/>
       <c r="R36" s="12"/>
@@ -2424,7 +2846,7 @@
       <c r="X36" s="12"/>
       <c r="AD36" s="13"/>
       <c r="AF36" s="9" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="AG36" s="34"/>
       <c r="AH36" s="35"/>
@@ -2432,26 +2854,26 @@
       <c r="AJ36" s="35"/>
       <c r="AK36" s="36"/>
       <c r="AL36" s="37"/>
-      <c r="AN36" s="56"/>
-      <c r="AO36" s="52"/>
-      <c r="AP36" s="52"/>
+      <c r="AN36" s="47"/>
+      <c r="AO36" s="46"/>
+      <c r="AP36" s="46"/>
       <c r="AQ36" s="12"/>
-      <c r="AU36" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV36" s="51"/>
-      <c r="AW36" s="51"/>
-      <c r="AX36" s="51"/>
-      <c r="AY36" s="51"/>
-      <c r="AZ36" s="51"/>
-      <c r="BA36" s="51"/>
+      <c r="AU36" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV36" s="62"/>
+      <c r="AW36" s="62"/>
+      <c r="AX36" s="62"/>
+      <c r="AY36" s="62"/>
+      <c r="AZ36" s="62"/>
+      <c r="BA36" s="62"/>
     </row>
     <row r="37" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>3</v>
@@ -2469,37 +2891,37 @@
         <v>9</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="48" t="s">
+      <c r="P37" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="49"/>
-      <c r="V37" s="50"/>
-      <c r="X37" s="56"/>
-      <c r="Y37" s="52"/>
-      <c r="Z37" s="52"/>
-      <c r="AA37" s="52"/>
-      <c r="AB37" s="52"/>
-      <c r="AC37" s="52"/>
-      <c r="AD37" s="60"/>
-      <c r="AF37" s="51" t="s">
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="59"/>
+      <c r="U37" s="59"/>
+      <c r="V37" s="60"/>
+      <c r="X37" s="47"/>
+      <c r="Y37" s="46"/>
+      <c r="Z37" s="46"/>
+      <c r="AA37" s="46"/>
+      <c r="AB37" s="46"/>
+      <c r="AC37" s="46"/>
+      <c r="AD37" s="51"/>
+      <c r="AF37" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AG37" s="51"/>
-      <c r="AH37" s="51"/>
-      <c r="AI37" s="51"/>
-      <c r="AJ37" s="51"/>
-      <c r="AK37" s="51"/>
-      <c r="AL37" s="51"/>
+      <c r="AG37" s="45"/>
+      <c r="AH37" s="45"/>
+      <c r="AI37" s="45"/>
+      <c r="AJ37" s="45"/>
+      <c r="AK37" s="45"/>
+      <c r="AL37" s="45"/>
       <c r="AQ37" s="12"/>
       <c r="AU37" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AV37" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="AW37" s="3" t="s">
         <v>3</v>
@@ -2521,10 +2943,16 @@
       <c r="A38" s="7">
         <v>1</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="26">
+        <v>45767</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="D38" s="11"/>
-      <c r="E38" s="10"/>
+      <c r="E38" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="F38" s="11"/>
       <c r="G38" s="5"/>
       <c r="L38" s="12"/>
@@ -2532,10 +2960,16 @@
       <c r="AU38" s="7">
         <v>1</v>
       </c>
-      <c r="AV38" s="26"/>
-      <c r="AW38" s="10"/>
+      <c r="AV38" s="26">
+        <v>45768</v>
+      </c>
+      <c r="AW38" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="AX38" s="11"/>
-      <c r="AY38" s="10"/>
+      <c r="AY38" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="AZ38" s="11"/>
       <c r="BA38" s="5"/>
     </row>
@@ -2543,48 +2977,60 @@
       <c r="A39" s="8">
         <v>2</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="12"/>
+      <c r="B39" s="27">
+        <v>45769</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D39" s="13"/>
-      <c r="E39" s="12"/>
+      <c r="E39" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="F39" s="13"/>
       <c r="G39" s="16"/>
       <c r="L39" s="12"/>
-      <c r="M39" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="N39" s="46"/>
-      <c r="O39" s="46"/>
-      <c r="P39" s="46"/>
-      <c r="Q39" s="46"/>
-      <c r="R39" s="46"/>
-      <c r="S39" s="47"/>
-      <c r="X39" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y39" s="51"/>
-      <c r="Z39" s="51"/>
-      <c r="AA39" s="51"/>
-      <c r="AB39" s="51"/>
-      <c r="AC39" s="51"/>
-      <c r="AD39" s="51"/>
-      <c r="AI39" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ39" s="51"/>
-      <c r="AK39" s="51"/>
-      <c r="AL39" s="51"/>
-      <c r="AM39" s="51"/>
-      <c r="AN39" s="51"/>
-      <c r="AO39" s="51"/>
+      <c r="M39" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="56"/>
+      <c r="S39" s="57"/>
+      <c r="X39" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="45"/>
+      <c r="AC39" s="45"/>
+      <c r="AD39" s="45"/>
+      <c r="AI39" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ39" s="56"/>
+      <c r="AK39" s="56"/>
+      <c r="AL39" s="56"/>
+      <c r="AM39" s="56"/>
+      <c r="AN39" s="56"/>
+      <c r="AO39" s="57"/>
       <c r="AQ39" s="12"/>
       <c r="AU39" s="8">
         <v>2</v>
       </c>
-      <c r="AV39" s="27"/>
-      <c r="AW39" s="12"/>
+      <c r="AV39" s="27">
+        <v>45770</v>
+      </c>
+      <c r="AW39" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="AX39" s="13"/>
-      <c r="AY39" s="12"/>
+      <c r="AY39" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="AZ39" s="13"/>
       <c r="BA39" s="16"/>
     </row>
@@ -2592,10 +3038,16 @@
       <c r="A40" s="8">
         <v>3</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="12"/>
+      <c r="B40" s="27">
+        <v>45772</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="D40" s="13"/>
-      <c r="E40" s="12"/>
+      <c r="E40" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="F40" s="13"/>
       <c r="G40" s="16"/>
       <c r="L40" s="12"/>
@@ -2603,7 +3055,7 @@
         <v>2</v>
       </c>
       <c r="N40" s="22" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="O40" s="22" t="s">
         <v>3</v>
@@ -2624,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="Y40" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="Z40" s="3" t="s">
         <v>3</v>
@@ -2645,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="AJ40" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="AK40" s="3" t="s">
         <v>3</v>
@@ -2666,10 +3118,16 @@
       <c r="AU40" s="8">
         <v>3</v>
       </c>
-      <c r="AV40" s="27"/>
-      <c r="AW40" s="12"/>
+      <c r="AV40" s="27">
+        <v>45772</v>
+      </c>
+      <c r="AW40" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="AX40" s="13"/>
-      <c r="AY40" s="12"/>
+      <c r="AY40" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="AZ40" s="13"/>
       <c r="BA40" s="16"/>
     </row>
@@ -2677,15 +3135,21 @@
       <c r="A41" s="8">
         <v>4</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="30"/>
+      <c r="B41" s="33">
+        <v>45774</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>23</v>
+      </c>
       <c r="D41" s="31"/>
-      <c r="E41" s="30"/>
+      <c r="E41" s="30" t="s">
+        <v>26</v>
+      </c>
       <c r="F41" s="31"/>
       <c r="G41" s="32"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
@@ -2714,27 +3178,39 @@
       <c r="AM41" s="23"/>
       <c r="AN41" s="24"/>
       <c r="AO41" s="25"/>
-      <c r="AQ41" s="56"/>
-      <c r="AR41" s="52"/>
-      <c r="AS41" s="52"/>
+      <c r="AQ41" s="47"/>
+      <c r="AR41" s="46"/>
+      <c r="AS41" s="46"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
-      <c r="AV41" s="33"/>
-      <c r="AW41" s="30"/>
+      <c r="AV41" s="33">
+        <v>45774</v>
+      </c>
+      <c r="AW41" s="30" t="s">
+        <v>34</v>
+      </c>
       <c r="AX41" s="31"/>
-      <c r="AY41" s="30"/>
+      <c r="AY41" s="30" t="s">
+        <v>33</v>
+      </c>
       <c r="AZ41" s="31"/>
       <c r="BA41" s="32"/>
     </row>
     <row r="42" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B42" s="27">
+        <v>45776</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D42" s="13"/>
-      <c r="E42" s="12"/>
+      <c r="E42" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="F42" s="13"/>
       <c r="G42" s="16"/>
       <c r="M42" s="8">
@@ -2765,23 +3241,35 @@
       <c r="AN42" s="13"/>
       <c r="AO42" s="16"/>
       <c r="AU42" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV42" s="27"/>
-      <c r="AW42" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="AV42" s="27">
+        <v>45776</v>
+      </c>
+      <c r="AW42" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="AX42" s="13"/>
-      <c r="AY42" s="12"/>
+      <c r="AY42" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="AZ42" s="13"/>
       <c r="BA42" s="16"/>
     </row>
     <row r="43" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="B43" s="27">
+        <v>45779</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="D43" s="13"/>
-      <c r="E43" s="12"/>
+      <c r="E43" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="F43" s="13"/>
       <c r="G43" s="16"/>
       <c r="M43" s="8">
@@ -2812,23 +3300,35 @@
       <c r="AN43" s="13"/>
       <c r="AO43" s="16"/>
       <c r="AU43" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AV43" s="27"/>
-      <c r="AW43" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="AV43" s="27">
+        <v>45778</v>
+      </c>
+      <c r="AW43" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="AX43" s="13"/>
-      <c r="AY43" s="12"/>
+      <c r="AY43" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="AZ43" s="13"/>
       <c r="BA43" s="32"/>
     </row>
     <row r="44" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="B44" s="28">
+        <v>45781</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="D44" s="15"/>
-      <c r="E44" s="14"/>
+      <c r="E44" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="F44" s="15"/>
       <c r="G44" s="6"/>
       <c r="M44" s="8">
@@ -2859,27 +3359,33 @@
       <c r="AN44" s="13"/>
       <c r="AO44" s="16"/>
       <c r="AU44" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV44" s="28"/>
-      <c r="AW44" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="AV44" s="28">
+        <v>45780</v>
+      </c>
+      <c r="AW44" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="AX44" s="15"/>
-      <c r="AY44" s="14"/>
+      <c r="AY44" s="14" t="s">
+        <v>34</v>
+      </c>
       <c r="AZ44" s="15"/>
       <c r="BA44" s="6"/>
     </row>
     <row r="45" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
       <c r="M45" s="8" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="12"/>
@@ -2897,7 +3403,7 @@
       <c r="AC45" s="13"/>
       <c r="AD45" s="16"/>
       <c r="AI45" s="8" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="AJ45" s="27"/>
       <c r="AK45" s="12"/>
@@ -2905,19 +3411,19 @@
       <c r="AM45" s="12"/>
       <c r="AN45" s="13"/>
       <c r="AO45" s="16"/>
-      <c r="AU45" s="51" t="s">
+      <c r="AU45" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AV45" s="51"/>
-      <c r="AW45" s="51"/>
-      <c r="AX45" s="51"/>
-      <c r="AY45" s="51"/>
-      <c r="AZ45" s="51"/>
-      <c r="BA45" s="51"/>
+      <c r="AV45" s="45"/>
+      <c r="AW45" s="45"/>
+      <c r="AX45" s="45"/>
+      <c r="AY45" s="45"/>
+      <c r="AZ45" s="45"/>
+      <c r="BA45" s="45"/>
     </row>
     <row r="46" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="N46" s="33"/>
       <c r="O46" s="12"/>
@@ -2935,7 +3441,7 @@
       <c r="AC46" s="13"/>
       <c r="AD46" s="16"/>
       <c r="AI46" s="8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="AJ46" s="27"/>
       <c r="AK46" s="12"/>
@@ -2945,8 +3451,8 @@
       <c r="AO46" s="16"/>
     </row>
     <row r="47" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M47" s="8" t="s">
-        <v>12</v>
+      <c r="M47" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="N47" s="34"/>
       <c r="O47" s="12"/>
@@ -2964,7 +3470,7 @@
       <c r="AC47" s="15"/>
       <c r="AD47" s="6"/>
       <c r="AI47" s="9" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="AJ47" s="28"/>
       <c r="AK47" s="14"/>
@@ -2974,49 +3480,61 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="45" t="s">
+      <c r="M48" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="N48" s="46"/>
-      <c r="O48" s="46"/>
-      <c r="P48" s="46"/>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="46"/>
-      <c r="S48" s="47"/>
-      <c r="X48" s="51" t="s">
+      <c r="N48" s="56"/>
+      <c r="O48" s="56"/>
+      <c r="P48" s="56"/>
+      <c r="Q48" s="56"/>
+      <c r="R48" s="56"/>
+      <c r="S48" s="57"/>
+      <c r="X48" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="Y48" s="51"/>
-      <c r="Z48" s="51"/>
-      <c r="AA48" s="51"/>
-      <c r="AB48" s="51"/>
-      <c r="AC48" s="51"/>
-      <c r="AD48" s="51"/>
-      <c r="AI48" s="51" t="s">
+      <c r="Y48" s="45"/>
+      <c r="Z48" s="45"/>
+      <c r="AA48" s="45"/>
+      <c r="AB48" s="45"/>
+      <c r="AC48" s="45"/>
+      <c r="AD48" s="45"/>
+      <c r="AI48" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AJ48" s="51"/>
-      <c r="AK48" s="51"/>
-      <c r="AL48" s="51"/>
-      <c r="AM48" s="51"/>
-      <c r="AN48" s="51"/>
-      <c r="AO48" s="51"/>
+      <c r="AJ48" s="45"/>
+      <c r="AK48" s="45"/>
+      <c r="AL48" s="45"/>
+      <c r="AM48" s="45"/>
+      <c r="AN48" s="45"/>
+      <c r="AO48" s="45"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="O26:W26"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="M4:S4"/>
+    <mergeCell ref="M13:S13"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="X37:AD37"/>
     <mergeCell ref="AE26:AM26"/>
     <mergeCell ref="Z1:AB1"/>
@@ -3033,30 +3551,18 @@
     <mergeCell ref="AN36:AP36"/>
     <mergeCell ref="AQ8:AS8"/>
     <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="O26:W26"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="M4:S4"/>
-    <mergeCell ref="M13:S13"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3067,25 +3573,25 @@
           <x14:formula1>
             <xm:f>Matchups!$A$14:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C11 E5:E11 I8:K8</xm:sqref>
+          <xm:sqref>I8:K8 E5:E11 C5:C11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$20:$A$21</xm:f>
           </x14:formula1>
-          <xm:sqref>C16:C22 E16:E22 I19:K19</xm:sqref>
+          <xm:sqref>I19:K19 C27:C33 E27:E33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$23:$A$24</xm:f>
           </x14:formula1>
-          <xm:sqref>C27:C33 E27:E33 I30:K30</xm:sqref>
+          <xm:sqref>I30:K30 C38:C44 E38:E44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$17:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>C38:C44 E38:E44 I41:K41</xm:sqref>
+          <xm:sqref>C16:C22 E16:E22 I41:K41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
@@ -3121,25 +3627,25 @@
           <x14:formula1>
             <xm:f>Matchups!$B$14:$B$15</xm:f>
           </x14:formula1>
-          <xm:sqref>AW5:AW11 AY5:AY11 AQ8:AS8</xm:sqref>
+          <xm:sqref>AQ8:AS8 AW5:AW11 AY5:AY11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$20:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>AW16:AW22 AY16:AY22 AQ19:AS19</xm:sqref>
+          <xm:sqref>AQ19:AS19 AW27:AW33 AY27:AY33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$23:$B$24</xm:f>
           </x14:formula1>
-          <xm:sqref>AW27:AW33 AY27:AY33 AQ30:AS30</xm:sqref>
+          <xm:sqref>AQ30:AS30 AW38:AW44 AY38:AY44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$17:$B$18</xm:f>
           </x14:formula1>
-          <xm:sqref>AW38:AW44 AY38:AY44 AQ41:AS41</xm:sqref>
+          <xm:sqref>AW16:AW22 AY16:AY22 AQ41:AS41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Updated Standings, Box Scores
Data Input to EOD 4/30/25
</commit_message>
<xml_diff>
--- a/2024_2025/Playoffs/Brackets.xlsx
+++ b/2024_2025/Playoffs/Brackets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024_2025\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024_2025\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F698CF-9DFC-401C-9DA7-C6FFD4F33456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="3" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="83">
   <si>
     <t>Game</t>
   </si>
@@ -266,12 +265,21 @@
   </si>
   <si>
     <t>Maple Leafs Lead 3-2</t>
+  </si>
+  <si>
+    <t>Capitals Win Series 4-1</t>
+  </si>
+  <si>
+    <t>Panthers Win Series 4-1</t>
+  </si>
+  <si>
+    <t>Jets Lead 3-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -647,30 +655,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -681,42 +725,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -998,11 +1006,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,22 +1026,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1058,7 +1066,9 @@
       <c r="B3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="D3" s="13"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1070,7 +1080,9 @@
       <c r="B4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="D4" s="13"/>
       <c r="E4" s="10"/>
       <c r="F4" s="17"/>
@@ -1085,7 +1097,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="65"/>
+      <c r="F5" s="44"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -1096,8 +1108,8 @@
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
@@ -1106,10 +1118,10 @@
       <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -1118,10 +1130,10 @@
       <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1130,24 +1142,24 @@
       <c r="B9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
     </row>
     <row r="10" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="43"/>
+      <c r="F10" s="48"/>
       <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1176,18 +1188,18 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="44" t="s">
+      <c r="D12" s="47"/>
+      <c r="E12" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="47"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1210,20 +1222,22 @@
       <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="45"/>
+      <c r="D15" s="47"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1232,7 +1246,9 @@
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1248,10 +1264,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="45"/>
+      <c r="B18" s="47"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1270,10 +1286,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="45"/>
+      <c r="B21" s="47"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1355,28 +1371,28 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:A14 A16:A17 A19:A20 A22:A23" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:A14 A16:A17 A19:A20 A22:A23">
       <formula1>$A$2:$A$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B14 B16:B17 B19:B20 B22:B23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B14 B16:B17 B19:B20 B22:B23">
       <formula1>$B$2:$B$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C14 C16:C17" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C14 C16:C17">
       <formula1>$C$2:$C$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D14 D16:D17" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D14 D16:D17">
       <formula1>$D$2:$D$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -1386,11 +1402,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AN14" sqref="AN14:AP14"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="BA10" sqref="BA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,124 +1453,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="57"/>
-      <c r="Z1" s="55" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="61"/>
+      <c r="Z1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="57"/>
-      <c r="AF1" s="55" t="s">
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="61"/>
+      <c r="AF1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="56"/>
-      <c r="AL1" s="56"/>
-      <c r="AM1" s="56"/>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="56"/>
-      <c r="AP1" s="56"/>
-      <c r="AQ1" s="56"/>
-      <c r="AR1" s="56"/>
-      <c r="AS1" s="56"/>
-      <c r="AT1" s="56"/>
-      <c r="AU1" s="56"/>
-      <c r="AV1" s="56"/>
-      <c r="AW1" s="56"/>
-      <c r="AX1" s="56"/>
-      <c r="AY1" s="56"/>
-      <c r="AZ1" s="56"/>
-      <c r="BA1" s="57"/>
+      <c r="AG1" s="60"/>
+      <c r="AH1" s="60"/>
+      <c r="AI1" s="60"/>
+      <c r="AJ1" s="60"/>
+      <c r="AK1" s="60"/>
+      <c r="AL1" s="60"/>
+      <c r="AM1" s="60"/>
+      <c r="AN1" s="60"/>
+      <c r="AO1" s="60"/>
+      <c r="AP1" s="60"/>
+      <c r="AQ1" s="60"/>
+      <c r="AR1" s="60"/>
+      <c r="AS1" s="60"/>
+      <c r="AT1" s="60"/>
+      <c r="AU1" s="60"/>
+      <c r="AV1" s="60"/>
+      <c r="AW1" s="60"/>
+      <c r="AX1" s="60"/>
+      <c r="AY1" s="60"/>
+      <c r="AZ1" s="60"/>
+      <c r="BA1" s="61"/>
     </row>
     <row r="2" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="M2" s="51" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="M2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="53"/>
-      <c r="AI2" s="51" t="s">
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="65"/>
+      <c r="AI2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="53"/>
-      <c r="AU2" s="51" t="s">
+      <c r="AJ2" s="64"/>
+      <c r="AK2" s="64"/>
+      <c r="AL2" s="64"/>
+      <c r="AM2" s="64"/>
+      <c r="AN2" s="64"/>
+      <c r="AO2" s="65"/>
+      <c r="AU2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="AV2" s="52"/>
-      <c r="AW2" s="52"/>
-      <c r="AX2" s="52"/>
-      <c r="AY2" s="52"/>
-      <c r="AZ2" s="52"/>
-      <c r="BA2" s="53"/>
+      <c r="AV2" s="64"/>
+      <c r="AW2" s="64"/>
+      <c r="AX2" s="64"/>
+      <c r="AY2" s="64"/>
+      <c r="AZ2" s="64"/>
+      <c r="BA2" s="65"/>
     </row>
     <row r="3" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="AI3" s="58" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="AI3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="59"/>
-      <c r="AL3" s="59"/>
-      <c r="AM3" s="59"/>
-      <c r="AN3" s="59"/>
-      <c r="AO3" s="60"/>
-      <c r="AU3" s="47" t="s">
+      <c r="AJ3" s="51"/>
+      <c r="AK3" s="51"/>
+      <c r="AL3" s="51"/>
+      <c r="AM3" s="51"/>
+      <c r="AN3" s="51"/>
+      <c r="AO3" s="52"/>
+      <c r="AU3" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="AV3" s="47"/>
-      <c r="AW3" s="47"/>
-      <c r="AX3" s="47"/>
-      <c r="AY3" s="47"/>
-      <c r="AZ3" s="47"/>
-      <c r="BA3" s="47"/>
+      <c r="AV3" s="57"/>
+      <c r="AW3" s="57"/>
+      <c r="AX3" s="57"/>
+      <c r="AY3" s="57"/>
+      <c r="AZ3" s="57"/>
+      <c r="BA3" s="57"/>
     </row>
     <row r="4" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -1578,15 +1594,15 @@
       <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="58" t="s">
+      <c r="M4" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="60"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="52"/>
       <c r="AI4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1856,9 +1872,9 @@
       <c r="H8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
@@ -1877,9 +1893,9 @@
       <c r="AM8" s="30"/>
       <c r="AN8" s="31"/>
       <c r="AO8" s="16"/>
-      <c r="AQ8" s="48"/>
-      <c r="AR8" s="48"/>
-      <c r="AS8" s="48"/>
+      <c r="AQ8" s="58"/>
+      <c r="AR8" s="58"/>
+      <c r="AS8" s="58"/>
       <c r="AU8" s="38">
         <v>4</v>
       </c>
@@ -1955,12 +1971,18 @@
       <c r="AW9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AX9" s="13"/>
+      <c r="AX9" s="13">
+        <v>3</v>
+      </c>
       <c r="AY9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AZ9" s="13"/>
-      <c r="BA9" s="32"/>
+      <c r="AZ9" s="13">
+        <v>5</v>
+      </c>
+      <c r="BA9" s="16" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -2067,15 +2089,15 @@
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
       <c r="L12" s="12"/>
       <c r="M12" s="9" t="s">
         <v>45</v>
@@ -2086,65 +2108,65 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="47" t="s">
+      <c r="AI12" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AJ12" s="47"/>
-      <c r="AK12" s="47"/>
-      <c r="AL12" s="47"/>
-      <c r="AM12" s="47"/>
-      <c r="AN12" s="47"/>
-      <c r="AO12" s="47"/>
+      <c r="AJ12" s="57"/>
+      <c r="AK12" s="57"/>
+      <c r="AL12" s="57"/>
+      <c r="AM12" s="57"/>
+      <c r="AN12" s="57"/>
+      <c r="AO12" s="57"/>
       <c r="AQ12" s="12"/>
-      <c r="AU12" s="47" t="s">
+      <c r="AU12" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AV12" s="47"/>
-      <c r="AW12" s="47"/>
-      <c r="AX12" s="47"/>
-      <c r="AY12" s="47"/>
-      <c r="AZ12" s="47"/>
-      <c r="BA12" s="47"/>
+      <c r="AV12" s="57"/>
+      <c r="AW12" s="57"/>
+      <c r="AX12" s="57"/>
+      <c r="AY12" s="57"/>
+      <c r="AZ12" s="57"/>
+      <c r="BA12" s="57"/>
     </row>
     <row r="13" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="58" t="s">
+      <c r="M13" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="60"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="52"/>
       <c r="AQ13" s="12"/>
     </row>
     <row r="14" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="AN14" s="48"/>
-      <c r="AO14" s="48"/>
-      <c r="AP14" s="48"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="AN14" s="58"/>
+      <c r="AO14" s="58"/>
+      <c r="AP14" s="58"/>
       <c r="AQ14" s="12"/>
-      <c r="AU14" s="50" t="s">
+      <c r="AU14" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="AV14" s="50"/>
-      <c r="AW14" s="50"/>
-      <c r="AX14" s="50"/>
-      <c r="AY14" s="50"/>
-      <c r="AZ14" s="50"/>
-      <c r="BA14" s="50"/>
+      <c r="AV14" s="56"/>
+      <c r="AW14" s="56"/>
+      <c r="AX14" s="56"/>
+      <c r="AY14" s="56"/>
+      <c r="AZ14" s="56"/>
+      <c r="BA14" s="56"/>
     </row>
     <row r="15" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2363,15 +2385,17 @@
       <c r="G19" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
+      <c r="I19" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="49"/>
-      <c r="AR19" s="48"/>
-      <c r="AS19" s="48"/>
+      <c r="AQ19" s="62"/>
+      <c r="AR19" s="58"/>
+      <c r="AS19" s="58"/>
       <c r="AU19" s="38">
         <v>4</v>
       </c>
@@ -2404,12 +2428,18 @@
       <c r="C20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="13">
+        <v>6</v>
+      </c>
       <c r="E20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="16"/>
+      <c r="F20" s="13">
+        <v>3</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>81</v>
+      </c>
       <c r="O20" s="12"/>
       <c r="AN20" s="12"/>
       <c r="AU20" s="8" t="s">
@@ -2503,52 +2533,52 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="47" t="s">
+      <c r="AU23" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AV23" s="47"/>
-      <c r="AW23" s="47"/>
-      <c r="AX23" s="47"/>
-      <c r="AY23" s="47"/>
-      <c r="AZ23" s="47"/>
-      <c r="BA23" s="47"/>
+      <c r="AV23" s="57"/>
+      <c r="AW23" s="57"/>
+      <c r="AX23" s="57"/>
+      <c r="AY23" s="57"/>
+      <c r="AZ23" s="57"/>
+      <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="47" t="s">
+      <c r="AU25" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="AV25" s="47"/>
-      <c r="AW25" s="47"/>
-      <c r="AX25" s="47"/>
-      <c r="AY25" s="47"/>
-      <c r="AZ25" s="47"/>
-      <c r="BA25" s="47"/>
+      <c r="AV25" s="57"/>
+      <c r="AW25" s="57"/>
+      <c r="AX25" s="57"/>
+      <c r="AY25" s="57"/>
+      <c r="AZ25" s="57"/>
+      <c r="BA25" s="57"/>
     </row>
     <row r="26" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
@@ -2572,24 +2602,24 @@
       <c r="G26" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="O26" s="49"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="48"/>
-      <c r="R26" s="48"/>
-      <c r="S26" s="48"/>
-      <c r="T26" s="48"/>
-      <c r="U26" s="48"/>
-      <c r="V26" s="48"/>
-      <c r="W26" s="48"/>
-      <c r="AE26" s="48"/>
-      <c r="AF26" s="48"/>
-      <c r="AG26" s="48"/>
-      <c r="AH26" s="48"/>
-      <c r="AI26" s="48"/>
-      <c r="AJ26" s="48"/>
-      <c r="AK26" s="48"/>
-      <c r="AL26" s="48"/>
-      <c r="AM26" s="54"/>
+      <c r="O26" s="62"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="AE26" s="58"/>
+      <c r="AF26" s="58"/>
+      <c r="AG26" s="58"/>
+      <c r="AH26" s="58"/>
+      <c r="AI26" s="58"/>
+      <c r="AJ26" s="58"/>
+      <c r="AK26" s="58"/>
+      <c r="AL26" s="58"/>
+      <c r="AM26" s="66"/>
       <c r="AU26" s="20" t="s">
         <v>0</v>
       </c>
@@ -2686,26 +2716,26 @@
         <v>61</v>
       </c>
       <c r="O28" s="12"/>
-      <c r="P28" s="58" t="s">
+      <c r="P28" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="59"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="60"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="52"/>
       <c r="X28" s="12"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="47" t="s">
+      <c r="AF28" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="AG28" s="47"/>
-      <c r="AH28" s="47"/>
-      <c r="AI28" s="47"/>
-      <c r="AJ28" s="47"/>
-      <c r="AK28" s="47"/>
-      <c r="AL28" s="47"/>
+      <c r="AG28" s="57"/>
+      <c r="AH28" s="57"/>
+      <c r="AI28" s="57"/>
+      <c r="AJ28" s="57"/>
+      <c r="AK28" s="57"/>
+      <c r="AL28" s="57"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
@@ -2841,9 +2871,11 @@
       <c r="G30" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
+      <c r="I30" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
@@ -2866,9 +2898,9 @@
       <c r="AK30" s="24"/>
       <c r="AL30" s="25"/>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="48"/>
-      <c r="AR30" s="48"/>
-      <c r="AS30" s="48"/>
+      <c r="AQ30" s="58"/>
+      <c r="AR30" s="58"/>
+      <c r="AS30" s="58"/>
       <c r="AU30" s="38">
         <v>4</v>
       </c>
@@ -2904,12 +2936,18 @@
       <c r="C31" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="13"/>
+      <c r="D31" s="13">
+        <v>1</v>
+      </c>
       <c r="E31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="32"/>
+      <c r="F31" s="13">
+        <v>4</v>
+      </c>
+      <c r="G31" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="L31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="8">
@@ -3074,15 +3112,15 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
@@ -3107,15 +3145,15 @@
       <c r="AL34" s="16"/>
       <c r="AN34" s="12"/>
       <c r="AQ34" s="12"/>
-      <c r="AU34" s="47" t="s">
+      <c r="AU34" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AV34" s="47"/>
-      <c r="AW34" s="47"/>
-      <c r="AX34" s="47"/>
-      <c r="AY34" s="47"/>
-      <c r="AZ34" s="47"/>
-      <c r="BA34" s="47"/>
+      <c r="AV34" s="57"/>
+      <c r="AW34" s="57"/>
+      <c r="AX34" s="57"/>
+      <c r="AY34" s="57"/>
+      <c r="AZ34" s="57"/>
+      <c r="BA34" s="57"/>
     </row>
     <row r="35" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
@@ -3144,18 +3182,18 @@
       <c r="AQ35" s="12"/>
     </row>
     <row r="36" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
       <c r="O36" s="12"/>
       <c r="P36" s="9" t="s">
         <v>45</v>
@@ -3177,19 +3215,19 @@
       <c r="AJ36" s="35"/>
       <c r="AK36" s="36"/>
       <c r="AL36" s="37"/>
-      <c r="AN36" s="49"/>
-      <c r="AO36" s="48"/>
-      <c r="AP36" s="48"/>
+      <c r="AN36" s="62"/>
+      <c r="AO36" s="58"/>
+      <c r="AP36" s="58"/>
       <c r="AQ36" s="12"/>
-      <c r="AU36" s="50" t="s">
+      <c r="AU36" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="AV36" s="50"/>
-      <c r="AW36" s="50"/>
-      <c r="AX36" s="50"/>
-      <c r="AY36" s="50"/>
-      <c r="AZ36" s="50"/>
-      <c r="BA36" s="50"/>
+      <c r="AV36" s="56"/>
+      <c r="AW36" s="56"/>
+      <c r="AX36" s="56"/>
+      <c r="AY36" s="56"/>
+      <c r="AZ36" s="56"/>
+      <c r="BA36" s="56"/>
     </row>
     <row r="37" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
@@ -3214,31 +3252,31 @@
         <v>7</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="61" t="s">
+      <c r="P37" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="Q37" s="62"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="62"/>
-      <c r="T37" s="62"/>
-      <c r="U37" s="62"/>
-      <c r="V37" s="63"/>
-      <c r="X37" s="49"/>
-      <c r="Y37" s="48"/>
-      <c r="Z37" s="48"/>
-      <c r="AA37" s="48"/>
-      <c r="AB37" s="48"/>
-      <c r="AC37" s="48"/>
-      <c r="AD37" s="54"/>
-      <c r="AF37" s="47" t="s">
+      <c r="Q37" s="54"/>
+      <c r="R37" s="54"/>
+      <c r="S37" s="54"/>
+      <c r="T37" s="54"/>
+      <c r="U37" s="54"/>
+      <c r="V37" s="55"/>
+      <c r="X37" s="62"/>
+      <c r="Y37" s="58"/>
+      <c r="Z37" s="58"/>
+      <c r="AA37" s="58"/>
+      <c r="AB37" s="58"/>
+      <c r="AC37" s="58"/>
+      <c r="AD37" s="66"/>
+      <c r="AF37" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AG37" s="47"/>
-      <c r="AH37" s="47"/>
-      <c r="AI37" s="47"/>
-      <c r="AJ37" s="47"/>
-      <c r="AK37" s="47"/>
-      <c r="AL37" s="47"/>
+      <c r="AG37" s="57"/>
+      <c r="AH37" s="57"/>
+      <c r="AI37" s="57"/>
+      <c r="AJ37" s="57"/>
+      <c r="AK37" s="57"/>
+      <c r="AL37" s="57"/>
       <c r="AQ37" s="12"/>
       <c r="AU37" s="3" t="s">
         <v>0</v>
@@ -3331,33 +3369,33 @@
         <v>58</v>
       </c>
       <c r="L39" s="12"/>
-      <c r="M39" s="58" t="s">
+      <c r="M39" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="60"/>
-      <c r="X39" s="47" t="s">
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="52"/>
+      <c r="X39" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="Y39" s="47"/>
-      <c r="Z39" s="47"/>
-      <c r="AA39" s="47"/>
-      <c r="AB39" s="47"/>
-      <c r="AC39" s="47"/>
-      <c r="AD39" s="47"/>
-      <c r="AI39" s="58" t="s">
+      <c r="Y39" s="57"/>
+      <c r="Z39" s="57"/>
+      <c r="AA39" s="57"/>
+      <c r="AB39" s="57"/>
+      <c r="AC39" s="57"/>
+      <c r="AD39" s="57"/>
+      <c r="AI39" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="AJ39" s="59"/>
-      <c r="AK39" s="59"/>
-      <c r="AL39" s="59"/>
-      <c r="AM39" s="59"/>
-      <c r="AN39" s="59"/>
-      <c r="AO39" s="60"/>
+      <c r="AJ39" s="51"/>
+      <c r="AK39" s="51"/>
+      <c r="AL39" s="51"/>
+      <c r="AM39" s="51"/>
+      <c r="AN39" s="51"/>
+      <c r="AO39" s="52"/>
       <c r="AQ39" s="12"/>
       <c r="AU39" s="8">
         <v>2</v>
@@ -3512,11 +3550,11 @@
       <c r="G41" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="48" t="s">
+      <c r="I41" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="58"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
@@ -3545,9 +3583,9 @@
       <c r="AM41" s="23"/>
       <c r="AN41" s="24"/>
       <c r="AO41" s="25"/>
-      <c r="AQ41" s="49"/>
-      <c r="AR41" s="48"/>
-      <c r="AS41" s="48"/>
+      <c r="AQ41" s="62"/>
+      <c r="AR41" s="58"/>
+      <c r="AS41" s="58"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
@@ -3763,15 +3801,15 @@
       <c r="BA44" s="6"/>
     </row>
     <row r="45" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
+      <c r="A45" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
       <c r="M45" s="8" t="s">
         <v>43</v>
       </c>
@@ -3799,15 +3837,15 @@
       <c r="AM45" s="12"/>
       <c r="AN45" s="13"/>
       <c r="AO45" s="16"/>
-      <c r="AU45" s="47" t="s">
+      <c r="AU45" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AV45" s="47"/>
-      <c r="AW45" s="47"/>
-      <c r="AX45" s="47"/>
-      <c r="AY45" s="47"/>
-      <c r="AZ45" s="47"/>
-      <c r="BA45" s="47"/>
+      <c r="AV45" s="57"/>
+      <c r="AW45" s="57"/>
+      <c r="AX45" s="57"/>
+      <c r="AY45" s="57"/>
+      <c r="AZ45" s="57"/>
+      <c r="BA45" s="57"/>
     </row>
     <row r="46" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
@@ -3868,45 +3906,65 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="58" t="s">
+      <c r="M48" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="N48" s="59"/>
-      <c r="O48" s="59"/>
-      <c r="P48" s="59"/>
-      <c r="Q48" s="59"/>
-      <c r="R48" s="59"/>
-      <c r="S48" s="60"/>
-      <c r="X48" s="47" t="s">
+      <c r="N48" s="51"/>
+      <c r="O48" s="51"/>
+      <c r="P48" s="51"/>
+      <c r="Q48" s="51"/>
+      <c r="R48" s="51"/>
+      <c r="S48" s="52"/>
+      <c r="X48" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="Y48" s="47"/>
-      <c r="Z48" s="47"/>
-      <c r="AA48" s="47"/>
-      <c r="AB48" s="47"/>
-      <c r="AC48" s="47"/>
-      <c r="AD48" s="47"/>
-      <c r="AI48" s="47" t="s">
+      <c r="Y48" s="57"/>
+      <c r="Z48" s="57"/>
+      <c r="AA48" s="57"/>
+      <c r="AB48" s="57"/>
+      <c r="AC48" s="57"/>
+      <c r="AD48" s="57"/>
+      <c r="AI48" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AJ48" s="47"/>
-      <c r="AK48" s="47"/>
-      <c r="AL48" s="47"/>
-      <c r="AM48" s="47"/>
-      <c r="AN48" s="47"/>
-      <c r="AO48" s="47"/>
+      <c r="AJ48" s="57"/>
+      <c r="AK48" s="57"/>
+      <c r="AL48" s="57"/>
+      <c r="AM48" s="57"/>
+      <c r="AN48" s="57"/>
+      <c r="AO48" s="57"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="X37:AD37"/>
+    <mergeCell ref="AE26:AM26"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="X39:AD39"/>
+    <mergeCell ref="X48:AD48"/>
+    <mergeCell ref="AF1:BA1"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="AI3:AO3"/>
+    <mergeCell ref="AI12:AO12"/>
+    <mergeCell ref="AI39:AO39"/>
+    <mergeCell ref="AU25:BA25"/>
+    <mergeCell ref="AI48:AO48"/>
+    <mergeCell ref="AN14:AP14"/>
+    <mergeCell ref="AN36:AP36"/>
+    <mergeCell ref="AQ8:AS8"/>
+    <mergeCell ref="AQ19:AS19"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="O26:W26"/>
     <mergeCell ref="I41:K41"/>
@@ -3923,125 +3981,105 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="A25:G25"/>
-    <mergeCell ref="X37:AD37"/>
-    <mergeCell ref="AE26:AM26"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="X39:AD39"/>
-    <mergeCell ref="X48:AD48"/>
-    <mergeCell ref="AF1:BA1"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="AI3:AO3"/>
-    <mergeCell ref="AI12:AO12"/>
-    <mergeCell ref="AI39:AO39"/>
-    <mergeCell ref="AU25:BA25"/>
-    <mergeCell ref="AI48:AO48"/>
-    <mergeCell ref="AN14:AP14"/>
-    <mergeCell ref="AN36:AP36"/>
-    <mergeCell ref="AQ8:AS8"/>
-    <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$13:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>I8:K8 C5:C11 E5:E11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$19:$A$20</xm:f>
           </x14:formula1>
           <xm:sqref>I30:K30 E27:E33 C27:C33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$22:$A$23</xm:f>
           </x14:formula1>
           <xm:sqref>C38:C44 I41:K41 E38:E44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$16:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>C16:C22 E16:E22 I19:K19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$C$13:$C$14</xm:f>
           </x14:formula1>
           <xm:sqref>L14:N14 O6:O12 Q6:Q12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$C$16:$C$17</xm:f>
           </x14:formula1>
           <xm:sqref>L36:N36 O41:O47 Q41:Q47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$E$13:$E$14</xm:f>
           </x14:formula1>
           <xm:sqref>T30:T36 R30:R36 O26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$F$13:$F$14</xm:f>
           </x14:formula1>
           <xm:sqref>AE26:AM26 AH30:AH36 AJ30:AJ36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$G$12:$G$13</xm:f>
           </x14:formula1>
           <xm:sqref>X37:AD37 AB41:AB47 Z41:Z47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$13:$B$14</xm:f>
           </x14:formula1>
           <xm:sqref>AQ8:AS8 AY5:AY11 AW5:AW11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$19:$B$20</xm:f>
           </x14:formula1>
           <xm:sqref>AQ30:AS30 AY27:AY33 AW27:AW33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$22:$B$23</xm:f>
           </x14:formula1>
           <xm:sqref>AQ41:AS41 AY38:AY44 AW38:AW44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$16:$B$17</xm:f>
           </x14:formula1>
           <xm:sqref>AW16:AW22 AY16:AY22 AQ19:AS19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$D$13:$D$14</xm:f>
           </x14:formula1>
           <xm:sqref>AN14:AP14 AM5:AM11 AK5:AK11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$D$16:$D$17</xm:f>
           </x14:formula1>

</xml_diff>